<commit_message>
Minor wording changes and fix brothers sorting bug
</commit_message>
<xml_diff>
--- a/src/data/fall19/bios_fall19.xlsx
+++ b/src/data/fall19/bios_fall19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farbodrafezy/Documents/personal/projects/dspuci-website-gatsby/src/data/fall19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD10C0-6A05-914A-B0CD-1DB7DF38561F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3A04C-7D00-FF41-9FA5-29F6CE1F2978}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -826,9 +826,6 @@
     <t xml:space="preserve">ASUCI Business Relations Commission, Indian Subcontinental Club </t>
   </si>
   <si>
-    <t>Traveling, Cooking, Hiking, Soccer, Journalling</t>
-  </si>
-  <si>
     <t>https://www.linkedin.com/in/malavikabasu</t>
   </si>
   <si>
@@ -1181,6 +1178,9 @@
   </si>
   <si>
     <t>Finance Intern at Experian in Costa Mesa, CA </t>
+  </si>
+  <si>
+    <t>Traveling, Cooking, Hiking, Soccer, Journaling</t>
   </si>
 </sst>
 </file>
@@ -1199,12 +1199,14 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1564,7 +1566,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1589,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1598,19 +1600,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>342</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>343</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>5</v>
@@ -1651,7 +1653,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>16</v>
@@ -1692,7 +1694,7 @@
         <v>24</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>25</v>
@@ -1736,7 +1738,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>35</v>
@@ -1777,7 +1779,7 @@
         <v>44</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>45</v>
@@ -1818,7 +1820,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>52</v>
@@ -1862,7 +1864,7 @@
         <v>59</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>60</v>
@@ -1906,7 +1908,7 @@
         <v>69</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>70</v>
@@ -1950,7 +1952,7 @@
         <v>79</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>80</v>
@@ -1991,7 +1993,7 @@
         <v>86</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>87</v>
@@ -2035,7 +2037,7 @@
         <v>95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>96</v>
@@ -2079,7 +2081,7 @@
         <v>103</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>104</v>
@@ -2123,7 +2125,7 @@
         <v>110</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>111</v>
@@ -2170,7 +2172,7 @@
         <v>119</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>35</v>
@@ -2211,7 +2213,7 @@
         <v>126</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>127</v>
@@ -2252,7 +2254,7 @@
         <v>132</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>133</v>
@@ -2293,7 +2295,7 @@
         <v>140</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>141</v>
@@ -2381,7 +2383,7 @@
         <v>140</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>157</v>
@@ -2422,7 +2424,7 @@
         <v>110</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>163</v>
@@ -2466,7 +2468,7 @@
         <v>170</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>171</v>
@@ -2507,7 +2509,7 @@
         <v>178</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>179</v>
@@ -2548,7 +2550,7 @@
         <v>184</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>185</v>
@@ -2595,7 +2597,7 @@
         <v>191</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>192</v>
@@ -2639,7 +2641,7 @@
         <v>110</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>198</v>
@@ -2680,7 +2682,7 @@
         <v>203</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>204</v>
@@ -2721,7 +2723,7 @@
         <v>210</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>211</v>
@@ -2765,7 +2767,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>216</v>
@@ -2806,7 +2808,7 @@
         <v>222</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>223</v>
@@ -2847,7 +2849,7 @@
         <v>230</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>231</v>
@@ -2891,7 +2893,7 @@
         <v>239</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>240</v>
@@ -2932,7 +2934,7 @@
         <v>245</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>246</v>
@@ -2976,7 +2978,7 @@
         <v>110</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>253</v>
@@ -3017,7 +3019,7 @@
         <v>110</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>259</v>
@@ -3061,19 +3063,19 @@
         <v>266</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>267</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>268</v>
+        <v>386</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>89</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3081,10 +3083,10 @@
         <v>43685.737630787036</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>155</v>
@@ -3102,22 +3104,22 @@
         <v>109</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="J36" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="K36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3125,10 +3127,10 @@
         <v>43711.585658518517</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>76</v>
@@ -3137,28 +3139,28 @@
         <v>67</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>139</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="J37" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="K37" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3166,10 +3168,10 @@
         <v>43710.56202484954</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>32</v>
@@ -3184,22 +3186,22 @@
         <v>78</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="J38" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="K38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>286</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>287</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3207,10 +3209,10 @@
         <v>43682.880619814816</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>289</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>290</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>32</v>
@@ -3219,7 +3221,7 @@
         <v>42</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>78</v>
@@ -3228,19 +3230,19 @@
         <v>170</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>293</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3248,10 +3250,10 @@
         <v>43682.890355752315</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>66</v>
@@ -3266,25 +3268,25 @@
         <v>14</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="J40" s="6" t="s">
-        <v>381</v>
-      </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>298</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>299</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N40" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="O40" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3292,7 +3294,7 @@
         <v>43684.30829612269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>40</v>
@@ -3310,22 +3312,22 @@
         <v>78</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3333,10 +3335,10 @@
         <v>43708.850029074078</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>92</v>
@@ -3345,34 +3347,34 @@
         <v>42</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N42" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="O42" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3380,10 +3382,10 @@
         <v>43710.987430995374</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>317</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>32</v>
@@ -3392,28 +3394,28 @@
         <v>12</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>139</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="J43" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3421,10 +3423,10 @@
         <v>43708.770285231483</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>76</v>
@@ -3433,31 +3435,31 @@
         <v>12</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="J44" s="6" t="s">
-        <v>385</v>
-      </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>330</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>113</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3465,10 +3467,10 @@
         <v>43683.611476053236</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>11</v>
@@ -3477,7 +3479,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>14</v>
@@ -3486,19 +3488,19 @@
         <v>95</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="L45" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>121</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add app part 1 to recruitment and update some bios
</commit_message>
<xml_diff>
--- a/src/data/fall19/bios_fall19.xlsx
+++ b/src/data/fall19/bios_fall19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/farbodrafezy/Documents/personal/projects/dspuci-website-gatsby/src/data/fall19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3A04C-7D00-FF41-9FA5-29F6CE1F2978}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A53FB3D-4398-744E-B55A-DF43F6676DDF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,9 +781,6 @@
     <t>Political Science</t>
   </si>
   <si>
-    <t>UCEAP Study Abroad in Milan, MAISS Peter Mentor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Traveling to new cities, surfing, reading, listening to podcasts, mentoring others </t>
   </si>
   <si>
@@ -1123,9 +1120,6 @@
     <t>Summer Financial Analyst at Wells Fargo Technology and Venture Banking in Irvine, CA </t>
   </si>
   <si>
-    <t>Administrative &amp; Marketing Intern at IvyBoost Education in Fremont, CA</t>
-  </si>
-  <si>
     <t>Credit Administration Intern at Pacific Premier Bank, Wealth Management Intern at Morgan Stanley, Accounting Intern at San Francisco Public Works </t>
   </si>
   <si>
@@ -1181,6 +1175,12 @@
   </si>
   <si>
     <t>Traveling, Cooking, Hiking, Soccer, Journaling</t>
+  </si>
+  <si>
+    <t>UCEAP Study Abroad in Milan, MAISS Mentor</t>
+  </si>
+  <si>
+    <t>Talent Acquisition Intern at Alliance HealthCare Services in Irvine, CA</t>
   </si>
 </sst>
 </file>
@@ -1563,10 +1563,10 @@
   <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L35" sqref="L35"/>
+      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1591,7 +1591,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>3</v>
@@ -1600,19 +1600,19 @@
         <v>4</v>
       </c>
       <c r="G1" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>339</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>340</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>341</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>342</v>
       </c>
       <c r="L1" s="4" t="s">
         <v>5</v>
@@ -1653,7 +1653,7 @@
         <v>15</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>16</v>
@@ -1694,7 +1694,7 @@
         <v>24</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>25</v>
@@ -1738,7 +1738,7 @@
         <v>15</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>35</v>
@@ -1779,7 +1779,7 @@
         <v>44</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>45</v>
@@ -1820,7 +1820,7 @@
         <v>15</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>52</v>
@@ -1864,7 +1864,7 @@
         <v>59</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>60</v>
@@ -1908,7 +1908,7 @@
         <v>69</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>70</v>
@@ -1952,7 +1952,7 @@
         <v>79</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>80</v>
@@ -1993,7 +1993,7 @@
         <v>86</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>87</v>
@@ -2037,7 +2037,7 @@
         <v>95</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>96</v>
@@ -2081,7 +2081,7 @@
         <v>103</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>104</v>
@@ -2125,7 +2125,7 @@
         <v>110</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>111</v>
@@ -2172,7 +2172,7 @@
         <v>119</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>35</v>
@@ -2213,7 +2213,7 @@
         <v>126</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>127</v>
@@ -2254,7 +2254,7 @@
         <v>132</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>133</v>
@@ -2295,7 +2295,7 @@
         <v>140</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>141</v>
@@ -2383,7 +2383,7 @@
         <v>140</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>157</v>
@@ -2424,7 +2424,7 @@
         <v>110</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>163</v>
@@ -2468,7 +2468,7 @@
         <v>170</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>171</v>
@@ -2509,7 +2509,7 @@
         <v>178</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>179</v>
@@ -2550,7 +2550,7 @@
         <v>184</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>185</v>
@@ -2597,7 +2597,7 @@
         <v>191</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>192</v>
@@ -2641,7 +2641,7 @@
         <v>110</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>198</v>
@@ -2682,7 +2682,7 @@
         <v>203</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>204</v>
@@ -2723,7 +2723,7 @@
         <v>210</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>367</v>
+        <v>386</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>211</v>
@@ -2767,7 +2767,7 @@
         <v>15</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>216</v>
@@ -2808,7 +2808,7 @@
         <v>222</v>
       </c>
       <c r="J29" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>223</v>
@@ -2849,7 +2849,7 @@
         <v>230</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>231</v>
@@ -2893,7 +2893,7 @@
         <v>239</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>240</v>
@@ -2934,7 +2934,7 @@
         <v>245</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>246</v>
@@ -2978,19 +2978,19 @@
         <v>110</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K33" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L33" s="2" t="s">
         <v>253</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>254</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N33" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2998,10 +2998,10 @@
         <v>43708.850521736109</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>257</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>66</v>
@@ -3010,7 +3010,7 @@
         <v>67</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>14</v>
@@ -3019,19 +3019,19 @@
         <v>110</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K34" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="L34" s="2" t="s">
         <v>259</v>
-      </c>
-      <c r="L34" s="2" t="s">
-        <v>260</v>
       </c>
       <c r="M34" s="2" t="s">
         <v>143</v>
       </c>
       <c r="N34" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3039,10 +3039,10 @@
         <v>43708.861152673606</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>262</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>263</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>155</v>
@@ -3051,31 +3051,31 @@
         <v>42</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H35" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="K35" s="2" t="s">
         <v>266</v>
       </c>
-      <c r="J35" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>267</v>
-      </c>
       <c r="L35" s="2" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>89</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3083,10 +3083,10 @@
         <v>43685.737630787036</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>269</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>270</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>155</v>
@@ -3104,22 +3104,22 @@
         <v>109</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>374</v>
+      </c>
+      <c r="K36" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="J36" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="K36" s="2" t="s">
+      <c r="L36" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>273</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>213</v>
       </c>
       <c r="N36" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3127,10 +3127,10 @@
         <v>43711.585658518517</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>76</v>
@@ -3139,28 +3139,28 @@
         <v>67</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>139</v>
       </c>
       <c r="I37" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="K37" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="J37" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="K37" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>280</v>
       </c>
       <c r="M37" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N37" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3168,10 +3168,10 @@
         <v>43710.56202484954</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>283</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>32</v>
@@ -3186,22 +3186,22 @@
         <v>78</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="K38" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="J38" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="K38" s="2" t="s">
+      <c r="L38" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="L38" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N38" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3209,10 +3209,10 @@
         <v>43682.880619814816</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>289</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>32</v>
@@ -3221,7 +3221,7 @@
         <v>42</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>78</v>
@@ -3230,19 +3230,19 @@
         <v>170</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K39" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="L39" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>292</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N39" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3250,10 +3250,10 @@
         <v>43682.890355752315</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>295</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>66</v>
@@ -3268,25 +3268,25 @@
         <v>14</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="K40" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="J40" s="6" t="s">
-        <v>380</v>
-      </c>
-      <c r="K40" s="2" t="s">
+      <c r="L40" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>298</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N40" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="O40" s="2" t="s">
         <v>299</v>
-      </c>
-      <c r="O40" s="2" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3294,7 +3294,7 @@
         <v>43684.30829612269</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>40</v>
@@ -3312,22 +3312,22 @@
         <v>78</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>35</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M41" s="2" t="s">
         <v>18</v>
       </c>
       <c r="N41" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3335,10 +3335,10 @@
         <v>43708.850029074078</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>92</v>
@@ -3347,34 +3347,34 @@
         <v>42</v>
       </c>
       <c r="F42" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="I42" s="2" t="s">
+      <c r="J42" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="K42" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="K42" s="2" t="s">
+      <c r="L42" s="2" t="s">
         <v>311</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>312</v>
       </c>
       <c r="M42" s="2" t="s">
         <v>47</v>
       </c>
       <c r="N42" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="O42" s="2" t="s">
         <v>313</v>
-      </c>
-      <c r="O42" s="2" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3382,10 +3382,10 @@
         <v>43710.987430995374</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>32</v>
@@ -3394,28 +3394,28 @@
         <v>12</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>139</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="K43" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="J43" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="K43" s="2" t="s">
+      <c r="L43" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="L43" s="2" t="s">
-        <v>320</v>
       </c>
       <c r="M43" s="2" t="s">
         <v>82</v>
       </c>
       <c r="N43" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3423,10 +3423,10 @@
         <v>43708.770285231483</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>322</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>323</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>76</v>
@@ -3435,31 +3435,31 @@
         <v>12</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="K44" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="J44" s="6" t="s">
-        <v>384</v>
-      </c>
-      <c r="K44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="L44" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="M44" s="2" t="s">
         <v>113</v>
       </c>
       <c r="N44" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3467,10 +3467,10 @@
         <v>43683.611476053236</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>331</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>332</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>11</v>
@@ -3479,7 +3479,7 @@
         <v>12</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>14</v>
@@ -3488,19 +3488,19 @@
         <v>95</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K45" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="L45" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="L45" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="M45" s="2" t="s">
         <v>121</v>
       </c>
       <c r="N45" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>